<commit_message>
compression img, amelioration accessibilite
</commit_message>
<xml_diff>
--- a/Audit_SEO_la_chouette_agence.xlsx
+++ b/Audit_SEO_la_chouette_agence.xlsx
@@ -8,18 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VnZnX\Desktop\Info\P4_Galpin_Vincent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1420E697-DD54-4A0A-9582-FA6425A11DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F59924A-3E7D-40C3-99A0-E1C20DD26E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="Feuil1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -32,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="114">
   <si>
     <t>Catégorie</t>
   </si>
@@ -371,6 +378,9 @@
   </si>
   <si>
     <t>Supprimer les éléments</t>
+  </si>
+  <si>
+    <t>//////////////////////////</t>
   </si>
 </sst>
 </file>
@@ -487,10 +497,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -723,13 +733,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" customWidth="1"/>
     <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="87.44140625" bestFit="1" customWidth="1"/>
@@ -790,7 +800,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>44</v>
       </c>
       <c r="B5" t="s">
@@ -810,7 +820,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+      <c r="A6" s="13"/>
       <c r="B6" t="s">
         <v>80</v>
       </c>
@@ -828,7 +838,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
+      <c r="A7" s="13"/>
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -846,7 +856,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
+      <c r="A8" s="13"/>
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -864,7 +874,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+      <c r="A9" s="13"/>
       <c r="B9" t="s">
         <v>16</v>
       </c>
@@ -882,11 +892,14 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="5" t="s">
+        <v>113</v>
+      </c>
       <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="14" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -906,7 +919,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
+      <c r="A12" s="14"/>
       <c r="B12" s="5" t="s">
         <v>23</v>
       </c>
@@ -921,7 +934,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="5" t="s">
         <v>53</v>
       </c>
@@ -939,7 +952,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
+      <c r="A14" s="14"/>
       <c r="B14" t="s">
         <v>85</v>
       </c>
@@ -958,7 +971,7 @@
       <c r="E15" s="11"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -978,14 +991,14 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="5" t="s">
         <v>31</v>
       </c>
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
+      <c r="A18" s="14"/>
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -993,7 +1006,7 @@
       <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="14" t="s">
         <v>32</v>
       </c>
       <c r="B20" t="s">
@@ -1010,7 +1023,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
+      <c r="A21" s="14"/>
       <c r="B21" s="5" t="s">
         <v>33</v>
       </c>
@@ -1023,7 +1036,7 @@
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
+      <c r="A22" s="14"/>
       <c r="B22" s="5" t="s">
         <v>33</v>
       </c>
@@ -1036,7 +1049,7 @@
       <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
+      <c r="A23" s="14"/>
       <c r="B23" t="s">
         <v>62</v>
       </c>
@@ -1051,11 +1064,11 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="13"/>
+      <c r="A24" s="14"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="13" t="s">
         <v>66</v>
       </c>
       <c r="B26" t="s">
@@ -1072,7 +1085,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
+      <c r="A27" s="13"/>
       <c r="B27" s="5" t="s">
         <v>67</v>
       </c>
@@ -1090,7 +1103,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
+      <c r="A28" s="13"/>
       <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1167,7 +1180,7 @@
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="13" t="s">
         <v>44</v>
       </c>
       <c r="B38" t="s">
@@ -1187,7 +1200,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
+      <c r="A39" s="13"/>
       <c r="B39" t="s">
         <v>7</v>
       </c>
@@ -1205,7 +1218,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
+      <c r="A40" s="13"/>
       <c r="B40" t="s">
         <v>10</v>
       </c>
@@ -1223,7 +1236,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
+      <c r="A41" s="13"/>
       <c r="B41" t="s">
         <v>16</v>
       </c>
@@ -1241,7 +1254,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
+      <c r="A42" s="13"/>
       <c r="B42" t="s">
         <v>80</v>
       </c>
@@ -1260,7 +1273,7 @@
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="14" t="s">
+      <c r="A44" s="13" t="s">
         <v>20</v>
       </c>
       <c r="B44" t="s">
@@ -1277,7 +1290,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="14"/>
+      <c r="A45" s="13"/>
       <c r="B45" t="s">
         <v>89</v>
       </c>
@@ -2324,13 +2337,13 @@
     <row r="1009" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="A26:A28"/>
     <mergeCell ref="A38:A42"/>
     <mergeCell ref="A11:A14"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A20:A24"/>
-    <mergeCell ref="A5:A10"/>
-    <mergeCell ref="A26:A28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F7" r:id="rId1" xr:uid="{31F88895-CA79-418C-B66F-1875DB59E9EA}"/>

</xml_diff>

<commit_message>
Retour du menu version mobile et du scrollToTop et correction appel JS CSS contact
</commit_message>
<xml_diff>
--- a/Audit_SEO_la_chouette_agence.xlsx
+++ b/Audit_SEO_la_chouette_agence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VnZnX\Desktop\Info\P4_Galpin_Vincent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F59924A-3E7D-40C3-99A0-E1C20DD26E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7296364-20B0-42A0-8F8D-5D64F22079D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="100">
   <si>
     <t>Catégorie</t>
   </si>
@@ -296,30 +296,6 @@
     <t>https://optimiz.me/choix-des-mots-cles-pour-le-referencement/</t>
   </si>
   <si>
-    <t>toggle navigation</t>
-  </si>
-  <si>
-    <t>aucune utiliter</t>
-  </si>
-  <si>
-    <t>Toggle de navigation sans utiliter avec un leger effet au survol</t>
-  </si>
-  <si>
-    <t>Supprimer</t>
-  </si>
-  <si>
-    <t>navbar</t>
-  </si>
-  <si>
-    <t>inutile</t>
-  </si>
-  <si>
-    <t>Liens vers page d'acceuil et vers la page 2 inutile, possibilité de revenir en page d'acceuil avec le logo</t>
-  </si>
-  <si>
-    <t>aucune utiliter + cacher 1ere page</t>
-  </si>
-  <si>
     <t>bloc 6</t>
   </si>
   <si>
@@ -338,9 +314,6 @@
     <t>bloc 7</t>
   </si>
   <si>
-    <t>balise label</t>
-  </si>
-  <si>
     <t>manque le label au formulaire</t>
   </si>
   <si>
@@ -350,37 +323,22 @@
     <t>https://www.alsacreations.com/astuce/lire/6-utiliser-element-label-input-formulaires.html</t>
   </si>
   <si>
-    <t>scrollbuton</t>
-  </si>
-  <si>
-    <t>bouton invisible</t>
-  </si>
-  <si>
-    <t>le bouton ne fonctionne pas</t>
-  </si>
-  <si>
     <t>Les balises label contiennent le formulaire</t>
   </si>
   <si>
-    <t>eviter de cacher des éléments</t>
-  </si>
-  <si>
-    <t>Suprrimer le bouton</t>
-  </si>
-  <si>
-    <t>Footer</t>
-  </si>
-  <si>
-    <t>identique a l'acceuil</t>
-  </si>
-  <si>
-    <t>beaucoup de code cacher</t>
-  </si>
-  <si>
-    <t>Supprimer les éléments</t>
-  </si>
-  <si>
     <t>//////////////////////////</t>
+  </si>
+  <si>
+    <t>script et css</t>
+  </si>
+  <si>
+    <t>erreur d'appelation JS et CSS</t>
+  </si>
+  <si>
+    <t>lier les bon fichiers au fichier html</t>
+  </si>
+  <si>
+    <t>balise aria label</t>
   </si>
 </sst>
 </file>
@@ -471,7 +429,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -501,6 +459,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -731,10 +692,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1009"/>
+  <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -894,7 +855,7 @@
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="5" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="E10" s="4"/>
     </row>
@@ -952,75 +913,73 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" t="s">
-        <v>85</v>
-      </c>
-      <c r="C14" t="s">
-        <v>92</v>
-      </c>
-      <c r="D14" t="s">
-        <v>87</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>88</v>
-      </c>
+      <c r="A14" s="9"/>
+      <c r="E14" s="11"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="E15" s="11"/>
+      <c r="A15" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>26</v>
-      </c>
+      <c r="A16" s="14"/>
       <c r="B16" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>57</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
-      <c r="B17" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
+      <c r="A18" s="7"/>
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="E19" s="4"/>
+      <c r="A19" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" t="s">
-        <v>63</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>64</v>
-      </c>
+      <c r="A20" s="14"/>
+      <c r="B20" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
@@ -1028,215 +987,214 @@
         <v>33</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
-      <c r="B22" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14"/>
-      <c r="B23" t="s">
+    </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" t="s">
         <v>62</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C25" t="s">
         <v>65</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D25" t="s">
         <v>63</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B26" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" t="s">
-        <v>65</v>
-      </c>
-      <c r="D26" t="s">
-        <v>63</v>
+      <c r="A26" s="13"/>
+      <c r="B26" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>64</v>
+        <v>56</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
-      <c r="B27" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>57</v>
-      </c>
+      <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
+      <c r="A28" s="10"/>
       <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
-      <c r="E29" s="4"/>
+      <c r="A29" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B30" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" t="s">
-        <v>70</v>
-      </c>
-      <c r="D30" t="s">
-        <v>71</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F30" s="12" t="s">
+      <c r="A30" s="10"/>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" t="s">
+        <v>75</v>
+      </c>
+      <c r="E31" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" s="12" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
-      <c r="E31" s="4"/>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
-        <v>73</v>
-      </c>
-      <c r="C32" t="s">
-        <v>74</v>
-      </c>
-      <c r="D32" t="s">
-        <v>75</v>
-      </c>
-      <c r="E32" t="s">
-        <v>76</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>13</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B33" t="s">
         <v>14</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C33" t="s">
         <v>15</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D33" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E33" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F34" s="12" t="s">
+      <c r="F33" s="12" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" t="s">
+        <v>46</v>
+      </c>
+      <c r="D37" t="s">
+        <v>47</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
-        <v>44</v>
-      </c>
+      <c r="A38" s="15"/>
       <c r="B38" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>47</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F38" s="12" t="s">
-        <v>58</v>
+        <v>9</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
+      <c r="A39" s="15"/>
       <c r="B39" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D39" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="15"/>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="C40" t="s">
-        <v>11</v>
+        <v>97</v>
       </c>
       <c r="D40" t="s">
-        <v>12</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
+      <c r="A41" s="15"/>
       <c r="B41" t="s">
         <v>16</v>
       </c>
@@ -1254,7 +1212,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
+      <c r="A42" s="15"/>
       <c r="B42" t="s">
         <v>80</v>
       </c>
@@ -1272,124 +1230,62 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B44" t="s">
+    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>85</v>
       </c>
-      <c r="C44" t="s">
+      <c r="B45" t="s">
         <v>86</v>
       </c>
-      <c r="D44" t="s">
+      <c r="C45" t="s">
         <v>87</v>
       </c>
-      <c r="E44" s="11" t="s">
+      <c r="D45" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="13"/>
-      <c r="B45" t="s">
+      <c r="E45" s="11" t="s">
         <v>89</v>
-      </c>
-      <c r="C45" t="s">
-        <v>90</v>
-      </c>
-      <c r="D45" t="s">
-        <v>91</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>90</v>
+      </c>
+      <c r="B47" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" t="s">
+        <v>91</v>
+      </c>
+      <c r="D47" t="s">
+        <v>94</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F47" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B47" t="s">
-        <v>94</v>
-      </c>
-      <c r="C47" t="s">
-        <v>95</v>
-      </c>
-      <c r="D47" t="s">
-        <v>96</v>
-      </c>
-      <c r="E47" s="11" t="s">
-        <v>97</v>
-      </c>
     </row>
     <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>98</v>
-      </c>
-      <c r="B49" t="s">
-        <v>99</v>
-      </c>
-      <c r="C49" t="s">
-        <v>100</v>
-      </c>
-      <c r="D49" t="s">
-        <v>106</v>
-      </c>
-      <c r="E49" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="F49" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>103</v>
-      </c>
-      <c r="B51" t="s">
-        <v>104</v>
-      </c>
-      <c r="C51" t="s">
-        <v>105</v>
-      </c>
-      <c r="D51" t="s">
-        <v>107</v>
-      </c>
-      <c r="E51" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>109</v>
-      </c>
-      <c r="B53" t="s">
-        <v>110</v>
-      </c>
-      <c r="C53" t="s">
-        <v>111</v>
-      </c>
-      <c r="D53" t="s">
-        <v>107</v>
-      </c>
-      <c r="E53" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2331,19 +2227,14 @@
     <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1006" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1007" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1008" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1009" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="6">
     <mergeCell ref="A5:A10"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="A37:A42"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F7" r:id="rId1" xr:uid="{31F88895-CA79-418C-B66F-1875DB59E9EA}"/>
@@ -2352,18 +2243,18 @@
     <hyperlink ref="F8" r:id="rId4" xr:uid="{465C3AE2-449F-411A-B576-41D4F92F21CD}"/>
     <hyperlink ref="F9" r:id="rId5" xr:uid="{76323957-333B-49DF-A642-B93DEBF40F68}"/>
     <hyperlink ref="F11" r:id="rId6" xr:uid="{7E3ADD3D-43B0-477D-9D86-0739DE06F813}"/>
-    <hyperlink ref="F16" r:id="rId7" xr:uid="{6C345C0E-6E0C-4336-AADC-A0888F70A399}"/>
-    <hyperlink ref="F27" r:id="rId8" xr:uid="{C8664034-CA90-4C5B-8C36-05DCE15B3129}"/>
-    <hyperlink ref="F30" r:id="rId9" xr:uid="{09831F82-A09E-49B0-974A-35C8E0D4D256}"/>
-    <hyperlink ref="F32" r:id="rId10" xr:uid="{A8366818-EAEC-4B93-B7C8-F9904D9D7869}"/>
-    <hyperlink ref="F34" r:id="rId11" xr:uid="{3016AA81-9F6C-4D78-A28F-73866791D9C8}"/>
-    <hyperlink ref="F39" r:id="rId12" xr:uid="{B4EDCC28-4E58-426E-BD25-992948E0C634}"/>
-    <hyperlink ref="F38" r:id="rId13" xr:uid="{C24268C3-C901-4BFD-89DC-627CEB744231}"/>
-    <hyperlink ref="F40" r:id="rId14" xr:uid="{A78A71F5-7E2C-4035-AC81-A05905FA0710}"/>
+    <hyperlink ref="F15" r:id="rId7" xr:uid="{6C345C0E-6E0C-4336-AADC-A0888F70A399}"/>
+    <hyperlink ref="F26" r:id="rId8" xr:uid="{C8664034-CA90-4C5B-8C36-05DCE15B3129}"/>
+    <hyperlink ref="F29" r:id="rId9" xr:uid="{09831F82-A09E-49B0-974A-35C8E0D4D256}"/>
+    <hyperlink ref="F31" r:id="rId10" xr:uid="{A8366818-EAEC-4B93-B7C8-F9904D9D7869}"/>
+    <hyperlink ref="F33" r:id="rId11" xr:uid="{3016AA81-9F6C-4D78-A28F-73866791D9C8}"/>
+    <hyperlink ref="F38" r:id="rId12" xr:uid="{B4EDCC28-4E58-426E-BD25-992948E0C634}"/>
+    <hyperlink ref="F37" r:id="rId13" xr:uid="{C24268C3-C901-4BFD-89DC-627CEB744231}"/>
+    <hyperlink ref="F39" r:id="rId14" xr:uid="{A78A71F5-7E2C-4035-AC81-A05905FA0710}"/>
     <hyperlink ref="F41" r:id="rId15" xr:uid="{9B07371E-E271-4A96-96A2-48A03142F2EA}"/>
     <hyperlink ref="F6" r:id="rId16" xr:uid="{E0DFE4AB-39B0-4052-8960-66BACEA0EE77}"/>
     <hyperlink ref="F42" r:id="rId17" xr:uid="{2AC04772-95A2-4B17-A5BB-4293F48E05F7}"/>
-    <hyperlink ref="F49" r:id="rId18" xr:uid="{2A5BF564-4798-4892-9B24-EF3B299F1E50}"/>
+    <hyperlink ref="F47" r:id="rId18" xr:uid="{2A5BF564-4798-4892-9B24-EF3B299F1E50}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId19"/>

</xml_diff>